<commit_message>
Sourced 0603 replacements for 0201 components
</commit_message>
<xml_diff>
--- a/Documents/Music_Visualizer_BOM.xlsx
+++ b/Documents/Music_Visualizer_BOM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ECE_Projects\Music_Visualizer\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E78EC930-D0B8-4BC8-A9BD-D9B69D46133E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9E37690-304C-434F-AB0F-477897FE129F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Music_Visualizer_BOM" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1015" uniqueCount="475">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1239" uniqueCount="644">
   <si>
     <t>Comment</t>
   </si>
@@ -1460,6 +1460,513 @@
   </si>
   <si>
     <t>https://www.digikey.ca/en/products/detail/taiyo-yuden/GMK105CC6105KV-F/13688729?s=N4IgTCBcDaIKwA4DsBaA4gWQNIEYAMcAwoQGz5xYBqKAYgCoBKKAcgCIgC6AvkA</t>
+  </si>
+  <si>
+    <t>1292-1445-1-ND</t>
+  </si>
+  <si>
+    <t>0603B473J250CT</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/en/products/detail/walsin-technology-corporation/0603B473J250CT/9354942</t>
+  </si>
+  <si>
+    <t>1292-1440-1-ND</t>
+  </si>
+  <si>
+    <t>0603B472J500CT</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/en/products/detail/walsin-technology-corporation/0603B472J500CT/9354937</t>
+  </si>
+  <si>
+    <t>1292-1521-1-ND</t>
+  </si>
+  <si>
+    <t>0603N332J500CT</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/en/products/detail/walsin-technology-corporation/0603N332J500CT/9355018</t>
+  </si>
+  <si>
+    <t>1276-1091-1-ND</t>
+  </si>
+  <si>
+    <t>CL10C102JB8NNNC</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/en/products/detail/samsung-electro-mechanics/CL10C102JB8NNNC/3886749</t>
+  </si>
+  <si>
+    <t>SMD: 0603</t>
+  </si>
+  <si>
+    <t>311-84.5KHRCT-ND</t>
+  </si>
+  <si>
+    <t>RC0603FR-0784K5L</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/en/products/detail/yageo/RC0603FR-0784K5L/727408</t>
+  </si>
+  <si>
+    <t>311-110KHRCT-ND</t>
+  </si>
+  <si>
+    <t>RC0603FR-07110KL</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/en/products/detail/yageo/RC0603FR-07110KL/726905</t>
+  </si>
+  <si>
+    <t>311-162KHRCT-ND</t>
+  </si>
+  <si>
+    <t>RC0603FR-07162KL</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/en/products/detail/yageo/RC0603FR-07162KL/726975</t>
+  </si>
+  <si>
+    <t>311-118KHRCT-ND</t>
+  </si>
+  <si>
+    <t>RC0603FR-07118KL</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/en/products/detail/yageo/RC0603FR-07118KL/726911</t>
+  </si>
+  <si>
+    <t>311-63.4KHRCT-ND</t>
+  </si>
+  <si>
+    <t>RC0603FR-0763K4L</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/en/products/detail/yageo/RC0603FR-0763K4L/727340</t>
+  </si>
+  <si>
+    <t>311-62.0KHRCT-ND</t>
+  </si>
+  <si>
+    <t>RC0603FR-0762KL</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/en/products/detail/yageo/RC0603FR-0762KL/727336</t>
+  </si>
+  <si>
+    <t>311-309KHRCT-ND</t>
+  </si>
+  <si>
+    <t>RC0603FR-07309KL</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/en/products/detail/yageo/RC0603FR-07309KL/727149</t>
+  </si>
+  <si>
+    <t>311-68.0KHRCT-ND</t>
+  </si>
+  <si>
+    <t>RC0603FR-0768KL</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/en/products/detail/yageo/RC0603FR-0768KL/727352</t>
+  </si>
+  <si>
+    <t>311-66.5KHRCT-ND</t>
+  </si>
+  <si>
+    <t>RC0603FR-0766K5L</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/en/products/detail/yageo/RC0603FR-0766K5L/727348</t>
+  </si>
+  <si>
+    <t>311-332KHRCT-ND</t>
+  </si>
+  <si>
+    <t>RC0603FR-07332KL</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/en/products/detail/yageo/RC0603FR-07332KL/727165</t>
+  </si>
+  <si>
+    <t>311-160KHRCT-ND</t>
+  </si>
+  <si>
+    <t>RC0603FR-07160KL</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/en/products/detail/yageo/RC0603FR-07160KL/726973</t>
+  </si>
+  <si>
+    <t>311-137KHRCT-ND</t>
+  </si>
+  <si>
+    <t>RC0603FR-07137KL</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/en/products/detail/yageo/RC0603FR-07137KL/726939</t>
+  </si>
+  <si>
+    <t>311-45.3KHRCT-ND</t>
+  </si>
+  <si>
+    <t>RC0603FR-0745K3L</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/en/products/detail/yageo/RC0603FR-0745K3L/727245</t>
+  </si>
+  <si>
+    <t>311-270KHRCT-ND</t>
+  </si>
+  <si>
+    <t>RC0603FR-07270KL</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/en/products/detail/yageo/RC0603FR-07270KL/727104</t>
+  </si>
+  <si>
+    <t>RMCF0603FT143KCT-ND</t>
+  </si>
+  <si>
+    <t>RMCF0603FT143K</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/en/products/detail/stackpole-electronics-inc/RMCF0603FT143K/1761301</t>
+  </si>
+  <si>
+    <t>311-19.1KHRCT-ND</t>
+  </si>
+  <si>
+    <t>RC0603FR-0719K1L</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/en/products/detail/yageo/RC0603FR-0719K1L/727001</t>
+  </si>
+  <si>
+    <t>311-590KHRCT-ND</t>
+  </si>
+  <si>
+    <t>RC0603FR-07590KL</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/en/products/detail/yageo/RC0603FR-07590KL/727315</t>
+  </si>
+  <si>
+    <t>311-140KHRCT-ND</t>
+  </si>
+  <si>
+    <t>RC0603FR-07140KL</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/en/products/detail/yageo/RC0603FR-07140KL/726947</t>
+  </si>
+  <si>
+    <t>311-18.7KHRCT-ND</t>
+  </si>
+  <si>
+    <t>RC0603FR-0718K7L</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/en/products/detail/yageo/RC0603FR-0718K7L/726993</t>
+  </si>
+  <si>
+    <t>311-576KHRCT-ND</t>
+  </si>
+  <si>
+    <t>RC0603FR-07576KL</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/en/products/detail/yageo/RC0603FR-07576KL/727311</t>
+  </si>
+  <si>
+    <t>311-100KHRCT-ND</t>
+  </si>
+  <si>
+    <t>RC0603FR-07100KL</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/en/products/detail/yageo/RC0603FR-07100KL/726889</t>
+  </si>
+  <si>
+    <t>311-169KHRCT-ND</t>
+  </si>
+  <si>
+    <t>RC0603FR-07169KL</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/en/products/detail/yageo/RC0603FR-07169KL/726979</t>
+  </si>
+  <si>
+    <t>311-33.2HRCT-ND</t>
+  </si>
+  <si>
+    <t>RC0603FR-0733R2L</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/en/products/detail/yageo/RC0603FR-0733R2L/727160</t>
+  </si>
+  <si>
+    <t>13-RC0603FR-1356KLCT-ND</t>
+  </si>
+  <si>
+    <t>RC0603FR-1356KL</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/en/products/detail/yageo/RC0603FR-1356KL/14286513</t>
+  </si>
+  <si>
+    <t>311-48.7KHRCT-ND</t>
+  </si>
+  <si>
+    <t>RC0603FR-0748K7L</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/en/products/detail/yageo/RC0603FR-0748K7L/727261</t>
+  </si>
+  <si>
+    <t>311-57.6KHRCT-ND</t>
+  </si>
+  <si>
+    <t>RC0603FR-0757K6L</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/en/products/detail/yageo/RC0603FR-0757K6L/727309</t>
+  </si>
+  <si>
+    <t>311-324KHRCT-ND</t>
+  </si>
+  <si>
+    <t>RC0603FR-07324KL</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/en/products/detail/yageo/RC0603FR-07324KL/727157</t>
+  </si>
+  <si>
+    <t>311-78.7KHRCT-ND</t>
+  </si>
+  <si>
+    <t>RC0603FR-0778K7L</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/en/products/detail/yageo/RC0603FR-0778K7L/727386</t>
+  </si>
+  <si>
+    <t>311-90.9KHRCT-ND</t>
+  </si>
+  <si>
+    <t>RC0603FR-0790K9L</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/en/products/detail/yageo/RC0603FR-0790K9L/727424</t>
+  </si>
+  <si>
+    <t>311-26.7KHRCT-ND</t>
+  </si>
+  <si>
+    <t>RC0603FR-0726K7L</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/en/products/detail/yageo/RC0603FR-0726K7L/727094</t>
+  </si>
+  <si>
+    <t>311-59.0KHRCT-ND</t>
+  </si>
+  <si>
+    <t>RC0603FR-0759KL</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/en/products/detail/yageo/RC0603FR-0759KL/727313</t>
+  </si>
+  <si>
+    <t>RC0603FR-077K87L</t>
+  </si>
+  <si>
+    <t>311-7.87KHRCT-ND</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/en/products/detail/yageo/RC0603FR-077K87L/727368</t>
+  </si>
+  <si>
+    <t>311-243KHRCT-ND</t>
+  </si>
+  <si>
+    <t>RC0603FR-07243KL</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/en/products/detail/yageo/RC0603FR-07243KL/727084</t>
+  </si>
+  <si>
+    <t>311-107KHRCT-ND</t>
+  </si>
+  <si>
+    <t>RC0603FR-07107KL</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/en/products/detail/yageo/RC0603FR-07107KL/726895</t>
+  </si>
+  <si>
+    <t>311-14.7KHRCT-ND</t>
+  </si>
+  <si>
+    <t>RC0603FR-0714K7L</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/en/products/detail/yageo/RC0603FR-0714K7L/726945</t>
+  </si>
+  <si>
+    <t>311-453KHRCT-ND</t>
+  </si>
+  <si>
+    <t>RC0603FR-07453KL</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/en/products/detail/yageo/RC0603FR-07453KL/727247</t>
+  </si>
+  <si>
+    <t>311-7.32KHRCT-ND</t>
+  </si>
+  <si>
+    <t>RC0603FR-077K32L</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/en/products/detail/yageo/RC0603FR-077K32L/727364</t>
+  </si>
+  <si>
+    <t>311-37.4KHRCT-ND</t>
+  </si>
+  <si>
+    <t>RC0603FR-0737K4L</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/en/products/detail/yageo/RC0603FR-0737K4L/727187</t>
+  </si>
+  <si>
+    <t>311-2.87KHRCT-ND</t>
+  </si>
+  <si>
+    <t>RC0603FR-072K87L</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/en/products/detail/yageo/RC0603FR-072K87L/727036</t>
+  </si>
+  <si>
+    <t>311-95.3KHRCT-ND</t>
+  </si>
+  <si>
+    <t>RC0603FR-0795K3L</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/en/products/detail/yageo/RC0603FR-0795K3L/727436</t>
+  </si>
+  <si>
+    <t>311-4.02KHRCT-ND</t>
+  </si>
+  <si>
+    <t>RC0603FR-074K02L</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/en/products/detail/yageo/RC0603FR-074K02L/727203</t>
+  </si>
+  <si>
+    <t>311-383KHRCT-ND</t>
+  </si>
+  <si>
+    <t>RC0603FR-07383KL</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/en/products/detail/yageo/RC0603FR-07383KL/727193</t>
+  </si>
+  <si>
+    <t>311-22.6KHRCT-ND</t>
+  </si>
+  <si>
+    <t>RC0603FR-0722K6L</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/en/products/detail/yageo/RC0603FR-0722K6L/727060</t>
+  </si>
+  <si>
+    <t>311-402KHRCT-ND</t>
+  </si>
+  <si>
+    <t>RC0603FR-07402KL</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/en/products/detail/yageo/RC0603FR-07402KL/727223</t>
+  </si>
+  <si>
+    <t>311-8.06KHRCT-ND</t>
+  </si>
+  <si>
+    <t>RC0603FR-078K06L</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/en/products/detail/yageo/RC0603FR-078K06L/727389</t>
+  </si>
+  <si>
+    <t>311-4.32KHRCT-ND</t>
+  </si>
+  <si>
+    <t>RC0603FR-074K32L</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/en/products/detail/yageo/RC0603FR-074K32L/727207</t>
+  </si>
+  <si>
+    <t>311-19.6KHRCT-ND</t>
+  </si>
+  <si>
+    <t>RC0603FR-0719K6L</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/en/products/detail/yageo/RC0603FR-0719K6L/727003</t>
+  </si>
+  <si>
+    <t>311-10.7KHRCT-ND</t>
+  </si>
+  <si>
+    <t>RC0603FR-0710K7L</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/en/products/detail/yageo/RC0603FR-0710K7L/726887</t>
+  </si>
+  <si>
+    <t>RNCP0603FTD1K00CT-ND</t>
+  </si>
+  <si>
+    <t>RNCP0603FTD1K00</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/en/products/detail/stackpole-electronics-inc/RNCP0603FTD1K00/2240106</t>
+  </si>
+  <si>
+    <t>YAG3330CT-ND</t>
+  </si>
+  <si>
+    <t>RC0603FR-0786R6L</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/en/products/detail/yageo/RC0603FR-0786R6L/5281190</t>
+  </si>
+  <si>
+    <t>311-35.7KHRCT-ND</t>
+  </si>
+  <si>
+    <t>RC0603FR-0735K7L</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/en/products/detail/yageo/RC0603FR-0735K7L/727175</t>
+  </si>
+  <si>
+    <t>311-390KHRCT-ND</t>
+  </si>
+  <si>
+    <t>RC0603FR-07390KL</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/en/products/detail/yageo/RC0603FR-07390KL/727199</t>
   </si>
 </sst>
 </file>
@@ -1469,7 +1976,7 @@
   <numFmts count="1">
     <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00;[Red]\-&quot;$&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1600,6 +2107,12 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -2309,7 +2822,7 @@
   <dimension ref="A1:I93"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5007,7 +5520,7 @@
   <dimension ref="A1:I57"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:I57"/>
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6679,14 +7192,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68457E54-D772-4DE5-8294-89212320B20A}">
   <dimension ref="A1:I57"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q11" sqref="Q11"/>
+    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
+      <selection activeCell="G60" sqref="G60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="23.77734375" customWidth="1"/>
     <col min="3" max="3" width="31.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
@@ -6725,11 +7240,28 @@
       <c r="B2" t="s">
         <v>10</v>
       </c>
+      <c r="C2" t="s">
+        <v>487</v>
+      </c>
       <c r="D2">
         <v>2</v>
       </c>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
+      <c r="E2" t="s">
+        <v>475</v>
+      </c>
+      <c r="F2" t="s">
+        <v>476</v>
+      </c>
+      <c r="G2" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="H2" s="1">
+        <f>D2*G2</f>
+        <v>0.2</v>
+      </c>
+      <c r="I2" t="s">
+        <v>477</v>
+      </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
@@ -6738,11 +7270,28 @@
       <c r="B3" t="s">
         <v>22</v>
       </c>
+      <c r="C3" t="s">
+        <v>487</v>
+      </c>
       <c r="D3">
         <v>2</v>
       </c>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
+      <c r="E3" t="s">
+        <v>478</v>
+      </c>
+      <c r="F3" t="s">
+        <v>479</v>
+      </c>
+      <c r="G3" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="H3" s="1">
+        <f>D3*G3</f>
+        <v>0.2</v>
+      </c>
+      <c r="I3" t="s">
+        <v>480</v>
+      </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
@@ -6751,11 +7300,28 @@
       <c r="B4" t="s">
         <v>27</v>
       </c>
+      <c r="C4" t="s">
+        <v>487</v>
+      </c>
       <c r="D4">
         <v>2</v>
       </c>
-      <c r="G4" s="1"/>
-      <c r="H4" s="1"/>
+      <c r="E4" t="s">
+        <v>481</v>
+      </c>
+      <c r="F4" t="s">
+        <v>482</v>
+      </c>
+      <c r="G4" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="H4" s="1">
+        <f>D4*G4</f>
+        <v>0.2</v>
+      </c>
+      <c r="I4" t="s">
+        <v>483</v>
+      </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
@@ -6764,11 +7330,28 @@
       <c r="B5" t="s">
         <v>43</v>
       </c>
+      <c r="C5" t="s">
+        <v>487</v>
+      </c>
       <c r="D5">
         <v>20</v>
       </c>
-      <c r="G5" s="1"/>
-      <c r="H5" s="1"/>
+      <c r="E5" t="s">
+        <v>484</v>
+      </c>
+      <c r="F5" t="s">
+        <v>485</v>
+      </c>
+      <c r="G5" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="H5" s="1">
+        <f>D5*G5</f>
+        <v>2</v>
+      </c>
+      <c r="I5" t="s">
+        <v>486</v>
+      </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
@@ -6777,11 +7360,28 @@
       <c r="B6" t="s">
         <v>133</v>
       </c>
+      <c r="C6" t="s">
+        <v>487</v>
+      </c>
       <c r="D6">
         <v>1</v>
       </c>
-      <c r="G6" s="1"/>
-      <c r="H6" s="1"/>
+      <c r="E6" t="s">
+        <v>488</v>
+      </c>
+      <c r="F6" t="s">
+        <v>489</v>
+      </c>
+      <c r="G6" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="H6" s="1">
+        <f>D6*G6</f>
+        <v>0.1</v>
+      </c>
+      <c r="I6" t="s">
+        <v>490</v>
+      </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
@@ -6790,11 +7390,28 @@
       <c r="B7" t="s">
         <v>139</v>
       </c>
+      <c r="C7" t="s">
+        <v>487</v>
+      </c>
       <c r="D7">
         <v>1</v>
       </c>
-      <c r="G7" s="1"/>
-      <c r="H7" s="1"/>
+      <c r="E7" t="s">
+        <v>491</v>
+      </c>
+      <c r="F7" t="s">
+        <v>492</v>
+      </c>
+      <c r="G7" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="H7" s="1">
+        <f>D7*G7</f>
+        <v>0.1</v>
+      </c>
+      <c r="I7" t="s">
+        <v>493</v>
+      </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
@@ -6803,11 +7420,28 @@
       <c r="B8" t="s">
         <v>144</v>
       </c>
+      <c r="C8" t="s">
+        <v>487</v>
+      </c>
       <c r="D8">
         <v>1</v>
       </c>
-      <c r="G8" s="1"/>
-      <c r="H8" s="1"/>
+      <c r="E8" t="s">
+        <v>494</v>
+      </c>
+      <c r="F8" t="s">
+        <v>495</v>
+      </c>
+      <c r="G8" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="H8" s="1">
+        <f>D8*G8</f>
+        <v>0.1</v>
+      </c>
+      <c r="I8" t="s">
+        <v>496</v>
+      </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
@@ -6816,11 +7450,28 @@
       <c r="B9" t="s">
         <v>149</v>
       </c>
+      <c r="C9" t="s">
+        <v>487</v>
+      </c>
       <c r="D9">
         <v>1</v>
       </c>
-      <c r="G9" s="1"/>
-      <c r="H9" s="1"/>
+      <c r="E9" t="s">
+        <v>497</v>
+      </c>
+      <c r="F9" t="s">
+        <v>498</v>
+      </c>
+      <c r="G9" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="H9" s="1">
+        <f>D9*G9</f>
+        <v>0.1</v>
+      </c>
+      <c r="I9" t="s">
+        <v>499</v>
+      </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
@@ -6829,11 +7480,28 @@
       <c r="B10" t="s">
         <v>154</v>
       </c>
+      <c r="C10" t="s">
+        <v>487</v>
+      </c>
       <c r="D10">
         <v>1</v>
       </c>
-      <c r="G10" s="1"/>
-      <c r="H10" s="1"/>
+      <c r="E10" t="s">
+        <v>500</v>
+      </c>
+      <c r="F10" t="s">
+        <v>501</v>
+      </c>
+      <c r="G10" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="H10" s="1">
+        <f>D10*G10</f>
+        <v>0.1</v>
+      </c>
+      <c r="I10" t="s">
+        <v>502</v>
+      </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
@@ -6842,11 +7510,28 @@
       <c r="B11" t="s">
         <v>159</v>
       </c>
+      <c r="C11" t="s">
+        <v>487</v>
+      </c>
       <c r="D11">
         <v>1</v>
       </c>
-      <c r="G11" s="1"/>
-      <c r="H11" s="1"/>
+      <c r="E11" t="s">
+        <v>503</v>
+      </c>
+      <c r="F11" t="s">
+        <v>504</v>
+      </c>
+      <c r="G11" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="H11" s="1">
+        <f>D11*G11</f>
+        <v>0.1</v>
+      </c>
+      <c r="I11" t="s">
+        <v>505</v>
+      </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
@@ -6855,11 +7540,28 @@
       <c r="B12" t="s">
         <v>164</v>
       </c>
+      <c r="C12" t="s">
+        <v>487</v>
+      </c>
       <c r="D12">
         <v>1</v>
       </c>
-      <c r="G12" s="1"/>
-      <c r="H12" s="1"/>
+      <c r="E12" t="s">
+        <v>506</v>
+      </c>
+      <c r="F12" t="s">
+        <v>507</v>
+      </c>
+      <c r="G12" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="H12" s="1">
+        <f>D12*G12</f>
+        <v>0.1</v>
+      </c>
+      <c r="I12" t="s">
+        <v>508</v>
+      </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
@@ -6868,11 +7570,28 @@
       <c r="B13" t="s">
         <v>169</v>
       </c>
+      <c r="C13" t="s">
+        <v>487</v>
+      </c>
       <c r="D13">
         <v>1</v>
       </c>
-      <c r="G13" s="1"/>
-      <c r="H13" s="1"/>
+      <c r="E13" t="s">
+        <v>509</v>
+      </c>
+      <c r="F13" t="s">
+        <v>510</v>
+      </c>
+      <c r="G13" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="H13" s="1">
+        <f>D13*G13</f>
+        <v>0.1</v>
+      </c>
+      <c r="I13" t="s">
+        <v>511</v>
+      </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
@@ -6881,11 +7600,28 @@
       <c r="B14" t="s">
         <v>174</v>
       </c>
+      <c r="C14" t="s">
+        <v>487</v>
+      </c>
       <c r="D14">
         <v>4</v>
       </c>
-      <c r="G14" s="1"/>
-      <c r="H14" s="1"/>
+      <c r="E14" t="s">
+        <v>512</v>
+      </c>
+      <c r="F14" t="s">
+        <v>513</v>
+      </c>
+      <c r="G14" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="H14" s="1">
+        <f t="shared" ref="H14:H26" si="0">D14*G14</f>
+        <v>0.4</v>
+      </c>
+      <c r="I14" t="s">
+        <v>514</v>
+      </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
@@ -6894,11 +7630,28 @@
       <c r="B15" t="s">
         <v>179</v>
       </c>
+      <c r="C15" t="s">
+        <v>487</v>
+      </c>
       <c r="D15">
         <v>1</v>
       </c>
-      <c r="G15" s="1"/>
-      <c r="H15" s="1"/>
+      <c r="E15" t="s">
+        <v>515</v>
+      </c>
+      <c r="F15" t="s">
+        <v>516</v>
+      </c>
+      <c r="G15" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="H15" s="1">
+        <f t="shared" si="0"/>
+        <v>0.1</v>
+      </c>
+      <c r="I15" t="s">
+        <v>517</v>
+      </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
@@ -6907,546 +7660,1262 @@
       <c r="B16" t="s">
         <v>184</v>
       </c>
+      <c r="C16" t="s">
+        <v>487</v>
+      </c>
       <c r="D16">
         <v>3</v>
       </c>
-      <c r="G16" s="1"/>
-      <c r="H16" s="1"/>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="E16" t="s">
+        <v>518</v>
+      </c>
+      <c r="F16" t="s">
+        <v>519</v>
+      </c>
+      <c r="G16" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="H16" s="1">
+        <f t="shared" si="0"/>
+        <v>0.30000000000000004</v>
+      </c>
+      <c r="I16" t="s">
+        <v>520</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>188</v>
       </c>
       <c r="B17" t="s">
         <v>189</v>
       </c>
+      <c r="C17" t="s">
+        <v>487</v>
+      </c>
       <c r="D17">
         <v>1</v>
       </c>
-      <c r="G17" s="1"/>
-      <c r="H17" s="1"/>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="E17" t="s">
+        <v>521</v>
+      </c>
+      <c r="F17" t="s">
+        <v>522</v>
+      </c>
+      <c r="G17" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="H17" s="1">
+        <f t="shared" si="0"/>
+        <v>0.1</v>
+      </c>
+      <c r="I17" t="s">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>193</v>
       </c>
       <c r="B18" t="s">
         <v>194</v>
       </c>
+      <c r="C18" t="s">
+        <v>487</v>
+      </c>
       <c r="D18">
         <v>1</v>
       </c>
-      <c r="G18" s="1"/>
-      <c r="H18" s="1"/>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="E18" t="s">
+        <v>524</v>
+      </c>
+      <c r="F18" t="s">
+        <v>525</v>
+      </c>
+      <c r="G18" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="H18" s="1">
+        <f t="shared" si="0"/>
+        <v>0.1</v>
+      </c>
+      <c r="I18" t="s">
+        <v>526</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>198</v>
       </c>
       <c r="B19" t="s">
         <v>199</v>
       </c>
+      <c r="C19" t="s">
+        <v>487</v>
+      </c>
       <c r="D19">
         <v>3</v>
       </c>
-      <c r="G19" s="1"/>
-      <c r="H19" s="1"/>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="E19" t="s">
+        <v>527</v>
+      </c>
+      <c r="F19" t="s">
+        <v>528</v>
+      </c>
+      <c r="G19" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="H19" s="1">
+        <f t="shared" si="0"/>
+        <v>0.30000000000000004</v>
+      </c>
+      <c r="I19" t="s">
+        <v>529</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>203</v>
       </c>
       <c r="B20" t="s">
         <v>204</v>
       </c>
+      <c r="C20" t="s">
+        <v>487</v>
+      </c>
       <c r="D20">
         <v>1</v>
       </c>
-      <c r="G20" s="1"/>
-      <c r="H20" s="1"/>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="E20" t="s">
+        <v>530</v>
+      </c>
+      <c r="F20" t="s">
+        <v>531</v>
+      </c>
+      <c r="G20" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="H20" s="1">
+        <f t="shared" si="0"/>
+        <v>0.1</v>
+      </c>
+      <c r="I20" t="s">
+        <v>532</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>208</v>
       </c>
       <c r="B21" t="s">
         <v>209</v>
       </c>
+      <c r="C21" t="s">
+        <v>487</v>
+      </c>
       <c r="D21">
         <v>1</v>
       </c>
-      <c r="G21" s="1"/>
-      <c r="H21" s="1"/>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="E21" t="s">
+        <v>533</v>
+      </c>
+      <c r="F21" t="s">
+        <v>534</v>
+      </c>
+      <c r="G21" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="H21" s="1">
+        <f t="shared" si="0"/>
+        <v>0.1</v>
+      </c>
+      <c r="I21" t="s">
+        <v>535</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>213</v>
       </c>
       <c r="B22" t="s">
         <v>214</v>
       </c>
+      <c r="C22" t="s">
+        <v>487</v>
+      </c>
       <c r="D22">
         <v>1</v>
       </c>
-      <c r="G22" s="1"/>
-      <c r="H22" s="1"/>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="E22" t="s">
+        <v>536</v>
+      </c>
+      <c r="F22" t="s">
+        <v>537</v>
+      </c>
+      <c r="G22" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="H22" s="1">
+        <f t="shared" si="0"/>
+        <v>0.1</v>
+      </c>
+      <c r="I22" t="s">
+        <v>538</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>218</v>
       </c>
       <c r="B23" t="s">
         <v>219</v>
       </c>
+      <c r="C23" t="s">
+        <v>487</v>
+      </c>
       <c r="D23">
         <v>1</v>
       </c>
-      <c r="G23" s="1"/>
-      <c r="H23" s="1"/>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="E23" t="s">
+        <v>539</v>
+      </c>
+      <c r="F23" t="s">
+        <v>540</v>
+      </c>
+      <c r="G23" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="H23" s="1">
+        <f t="shared" si="0"/>
+        <v>0.1</v>
+      </c>
+      <c r="I23" t="s">
+        <v>541</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>223</v>
       </c>
       <c r="B24" t="s">
         <v>224</v>
       </c>
+      <c r="C24" t="s">
+        <v>487</v>
+      </c>
       <c r="D24">
         <v>1</v>
       </c>
-      <c r="G24" s="1"/>
-      <c r="H24" s="1"/>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="E24" t="s">
+        <v>542</v>
+      </c>
+      <c r="F24" t="s">
+        <v>543</v>
+      </c>
+      <c r="G24" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="H24" s="1">
+        <f t="shared" si="0"/>
+        <v>0.1</v>
+      </c>
+      <c r="I24" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>228</v>
       </c>
       <c r="B25" t="s">
         <v>229</v>
       </c>
+      <c r="C25" t="s">
+        <v>487</v>
+      </c>
       <c r="D25">
         <v>1</v>
       </c>
-      <c r="G25" s="1"/>
-      <c r="H25" s="1"/>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="E25" t="s">
+        <v>545</v>
+      </c>
+      <c r="F25" t="s">
+        <v>546</v>
+      </c>
+      <c r="G25" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="H25" s="1">
+        <f t="shared" si="0"/>
+        <v>0.1</v>
+      </c>
+      <c r="I25" t="s">
+        <v>547</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>233</v>
       </c>
       <c r="B26" t="s">
         <v>234</v>
       </c>
+      <c r="C26" t="s">
+        <v>487</v>
+      </c>
       <c r="D26">
         <v>2</v>
       </c>
-      <c r="G26" s="1"/>
-      <c r="H26" s="1"/>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="E26" t="s">
+        <v>548</v>
+      </c>
+      <c r="F26" t="s">
+        <v>549</v>
+      </c>
+      <c r="G26" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="H26" s="1">
+        <f>D26*G26</f>
+        <v>0.2</v>
+      </c>
+      <c r="I26" t="s">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>238</v>
       </c>
       <c r="B27" t="s">
         <v>239</v>
       </c>
+      <c r="C27" t="s">
+        <v>487</v>
+      </c>
       <c r="D27">
         <v>1</v>
       </c>
-      <c r="G27" s="1"/>
-      <c r="H27" s="1"/>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="E27" t="s">
+        <v>551</v>
+      </c>
+      <c r="F27" t="s">
+        <v>552</v>
+      </c>
+      <c r="G27" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="H27" s="1">
+        <f>D27*G27</f>
+        <v>0.1</v>
+      </c>
+      <c r="I27" t="s">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>243</v>
       </c>
       <c r="B28" t="s">
         <v>244</v>
       </c>
+      <c r="C28" t="s">
+        <v>487</v>
+      </c>
       <c r="D28">
         <v>1</v>
       </c>
-      <c r="G28" s="1"/>
-      <c r="H28" s="1"/>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="E28" t="s">
+        <v>554</v>
+      </c>
+      <c r="F28" t="s">
+        <v>555</v>
+      </c>
+      <c r="G28" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="H28" s="1">
+        <f t="shared" ref="H28:H57" si="1">D28*G28</f>
+        <v>0.1</v>
+      </c>
+      <c r="I28" t="s">
+        <v>556</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>248</v>
       </c>
       <c r="B29" t="s">
         <v>249</v>
       </c>
+      <c r="C29" t="s">
+        <v>487</v>
+      </c>
       <c r="D29">
         <v>1</v>
       </c>
-      <c r="G29" s="1"/>
-      <c r="H29" s="1"/>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="E29" t="s">
+        <v>557</v>
+      </c>
+      <c r="F29" t="s">
+        <v>558</v>
+      </c>
+      <c r="G29" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="H29" s="1">
+        <f t="shared" si="1"/>
+        <v>0.1</v>
+      </c>
+      <c r="I29" t="s">
+        <v>559</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>253</v>
       </c>
       <c r="B30" t="s">
         <v>254</v>
       </c>
+      <c r="C30" t="s">
+        <v>487</v>
+      </c>
       <c r="D30">
         <v>2</v>
       </c>
-      <c r="G30" s="1"/>
-      <c r="H30" s="1"/>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="E30" t="s">
+        <v>560</v>
+      </c>
+      <c r="F30" t="s">
+        <v>561</v>
+      </c>
+      <c r="G30" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="H30" s="1">
+        <f t="shared" si="1"/>
+        <v>0.2</v>
+      </c>
+      <c r="I30" t="s">
+        <v>562</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>258</v>
       </c>
       <c r="B31" t="s">
         <v>259</v>
       </c>
+      <c r="C31" t="s">
+        <v>487</v>
+      </c>
       <c r="D31">
         <v>1</v>
       </c>
-      <c r="G31" s="1"/>
-      <c r="H31" s="1"/>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="E31" t="s">
+        <v>563</v>
+      </c>
+      <c r="F31" t="s">
+        <v>564</v>
+      </c>
+      <c r="G31" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="H31" s="1">
+        <f t="shared" si="1"/>
+        <v>0.1</v>
+      </c>
+      <c r="I31" t="s">
+        <v>565</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>263</v>
       </c>
       <c r="B32" t="s">
         <v>264</v>
       </c>
+      <c r="C32" t="s">
+        <v>487</v>
+      </c>
       <c r="D32">
         <v>1</v>
       </c>
-      <c r="G32" s="1"/>
-      <c r="H32" s="1"/>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="E32" t="s">
+        <v>566</v>
+      </c>
+      <c r="F32" t="s">
+        <v>567</v>
+      </c>
+      <c r="G32" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="H32" s="1">
+        <f t="shared" si="1"/>
+        <v>0.1</v>
+      </c>
+      <c r="I32" t="s">
+        <v>568</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>268</v>
       </c>
       <c r="B33" t="s">
         <v>269</v>
       </c>
+      <c r="C33" t="s">
+        <v>487</v>
+      </c>
       <c r="D33">
         <v>2</v>
       </c>
-      <c r="G33" s="1"/>
-      <c r="H33" s="1"/>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="E33" t="s">
+        <v>569</v>
+      </c>
+      <c r="F33" t="s">
+        <v>570</v>
+      </c>
+      <c r="G33" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="H33" s="1">
+        <f t="shared" si="1"/>
+        <v>0.2</v>
+      </c>
+      <c r="I33" t="s">
+        <v>571</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>273</v>
       </c>
       <c r="B34" t="s">
         <v>274</v>
       </c>
+      <c r="C34" t="s">
+        <v>487</v>
+      </c>
       <c r="D34">
         <v>3</v>
       </c>
-      <c r="G34" s="1"/>
-      <c r="H34" s="1"/>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="E34" t="s">
+        <v>572</v>
+      </c>
+      <c r="F34" t="s">
+        <v>573</v>
+      </c>
+      <c r="G34" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="H34" s="1">
+        <f t="shared" si="1"/>
+        <v>0.30000000000000004</v>
+      </c>
+      <c r="I34" t="s">
+        <v>574</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>278</v>
       </c>
       <c r="B35" t="s">
         <v>279</v>
       </c>
+      <c r="C35" t="s">
+        <v>487</v>
+      </c>
       <c r="D35">
         <v>1</v>
       </c>
-      <c r="G35" s="1"/>
-      <c r="H35" s="1"/>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="E35" t="s">
+        <v>575</v>
+      </c>
+      <c r="F35" t="s">
+        <v>576</v>
+      </c>
+      <c r="G35" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="H35" s="1">
+        <f t="shared" si="1"/>
+        <v>0.1</v>
+      </c>
+      <c r="I35" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>283</v>
       </c>
       <c r="B36" t="s">
         <v>284</v>
       </c>
+      <c r="C36" t="s">
+        <v>487</v>
+      </c>
       <c r="D36">
         <v>1</v>
       </c>
-      <c r="G36" s="1"/>
-      <c r="H36" s="1"/>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="E36" t="s">
+        <v>578</v>
+      </c>
+      <c r="F36" t="s">
+        <v>579</v>
+      </c>
+      <c r="G36" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="H36" s="1">
+        <f t="shared" si="1"/>
+        <v>0.1</v>
+      </c>
+      <c r="I36" t="s">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>288</v>
       </c>
       <c r="B37" t="s">
         <v>289</v>
       </c>
+      <c r="C37" t="s">
+        <v>487</v>
+      </c>
       <c r="D37">
         <v>1</v>
       </c>
-      <c r="G37" s="1"/>
-      <c r="H37" s="1"/>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="E37" t="s">
+        <v>582</v>
+      </c>
+      <c r="F37" t="s">
+        <v>581</v>
+      </c>
+      <c r="G37" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="H37" s="1">
+        <f t="shared" si="1"/>
+        <v>0.1</v>
+      </c>
+      <c r="I37" t="s">
+        <v>583</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>293</v>
       </c>
       <c r="B38" t="s">
         <v>294</v>
       </c>
+      <c r="C38" t="s">
+        <v>487</v>
+      </c>
       <c r="D38">
         <v>1</v>
       </c>
-      <c r="G38" s="1"/>
-      <c r="H38" s="1"/>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="E38" t="s">
+        <v>584</v>
+      </c>
+      <c r="F38" t="s">
+        <v>585</v>
+      </c>
+      <c r="G38" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="H38" s="1">
+        <f t="shared" si="1"/>
+        <v>0.1</v>
+      </c>
+      <c r="I38" t="s">
+        <v>586</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>298</v>
       </c>
       <c r="B39" t="s">
         <v>299</v>
       </c>
+      <c r="C39" t="s">
+        <v>487</v>
+      </c>
       <c r="D39">
         <v>1</v>
       </c>
-      <c r="G39" s="1"/>
-      <c r="H39" s="1"/>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="E39" t="s">
+        <v>587</v>
+      </c>
+      <c r="F39" t="s">
+        <v>588</v>
+      </c>
+      <c r="G39" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="H39" s="1">
+        <f t="shared" si="1"/>
+        <v>0.1</v>
+      </c>
+      <c r="I39" t="s">
+        <v>589</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>303</v>
       </c>
       <c r="B40" t="s">
         <v>304</v>
       </c>
+      <c r="C40" t="s">
+        <v>487</v>
+      </c>
       <c r="D40">
         <v>1</v>
       </c>
-      <c r="G40" s="1"/>
-      <c r="H40" s="1"/>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="E40" t="s">
+        <v>590</v>
+      </c>
+      <c r="F40" t="s">
+        <v>591</v>
+      </c>
+      <c r="G40" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="H40" s="1">
+        <f t="shared" si="1"/>
+        <v>0.1</v>
+      </c>
+      <c r="I40" t="s">
+        <v>592</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>308</v>
       </c>
       <c r="B41" t="s">
         <v>309</v>
       </c>
+      <c r="C41" t="s">
+        <v>487</v>
+      </c>
       <c r="D41">
         <v>1</v>
       </c>
-      <c r="G41" s="1"/>
-      <c r="H41" s="1"/>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="E41" t="s">
+        <v>593</v>
+      </c>
+      <c r="F41" t="s">
+        <v>594</v>
+      </c>
+      <c r="G41" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="H41" s="1">
+        <f t="shared" si="1"/>
+        <v>0.1</v>
+      </c>
+      <c r="I41" t="s">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>313</v>
       </c>
       <c r="B42" t="s">
         <v>314</v>
       </c>
+      <c r="C42" t="s">
+        <v>487</v>
+      </c>
       <c r="D42">
         <v>1</v>
       </c>
-      <c r="G42" s="1"/>
-      <c r="H42" s="1"/>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="E42" t="s">
+        <v>596</v>
+      </c>
+      <c r="F42" t="s">
+        <v>597</v>
+      </c>
+      <c r="G42" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="H42" s="1">
+        <f t="shared" si="1"/>
+        <v>0.1</v>
+      </c>
+      <c r="I42" t="s">
+        <v>598</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>318</v>
       </c>
       <c r="B43" t="s">
         <v>319</v>
       </c>
+      <c r="C43" t="s">
+        <v>487</v>
+      </c>
       <c r="D43">
         <v>2</v>
       </c>
-      <c r="G43" s="1"/>
-      <c r="H43" s="1"/>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="E43" t="s">
+        <v>599</v>
+      </c>
+      <c r="F43" t="s">
+        <v>600</v>
+      </c>
+      <c r="G43" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="H43" s="1">
+        <f t="shared" si="1"/>
+        <v>0.2</v>
+      </c>
+      <c r="I43" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>323</v>
       </c>
       <c r="B44" t="s">
         <v>324</v>
       </c>
+      <c r="C44" t="s">
+        <v>487</v>
+      </c>
       <c r="D44">
         <v>1</v>
       </c>
-      <c r="G44" s="1"/>
-      <c r="H44" s="1"/>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="E44" t="s">
+        <v>602</v>
+      </c>
+      <c r="F44" t="s">
+        <v>603</v>
+      </c>
+      <c r="G44" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="H44" s="1">
+        <f t="shared" si="1"/>
+        <v>0.1</v>
+      </c>
+      <c r="I44" t="s">
+        <v>604</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>328</v>
       </c>
       <c r="B45" t="s">
         <v>329</v>
       </c>
+      <c r="C45" t="s">
+        <v>487</v>
+      </c>
       <c r="D45">
         <v>1</v>
       </c>
-      <c r="G45" s="1"/>
-      <c r="H45" s="1"/>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="E45" t="s">
+        <v>605</v>
+      </c>
+      <c r="F45" t="s">
+        <v>606</v>
+      </c>
+      <c r="G45" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="H45" s="1">
+        <f t="shared" si="1"/>
+        <v>0.1</v>
+      </c>
+      <c r="I45" t="s">
+        <v>607</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>333</v>
       </c>
       <c r="B46" t="s">
         <v>334</v>
       </c>
+      <c r="C46" t="s">
+        <v>487</v>
+      </c>
       <c r="D46">
         <v>1</v>
       </c>
-      <c r="G46" s="1"/>
-      <c r="H46" s="1"/>
-    </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="E46" t="s">
+        <v>608</v>
+      </c>
+      <c r="F46" t="s">
+        <v>609</v>
+      </c>
+      <c r="G46" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="H46" s="1">
+        <f t="shared" si="1"/>
+        <v>0.1</v>
+      </c>
+      <c r="I46" t="s">
+        <v>610</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>338</v>
       </c>
       <c r="B47" t="s">
         <v>339</v>
       </c>
+      <c r="C47" t="s">
+        <v>487</v>
+      </c>
       <c r="D47">
         <v>1</v>
       </c>
-      <c r="G47" s="1"/>
-      <c r="H47" s="1"/>
-    </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="E47" t="s">
+        <v>611</v>
+      </c>
+      <c r="F47" t="s">
+        <v>612</v>
+      </c>
+      <c r="G47" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="H47" s="1">
+        <f t="shared" si="1"/>
+        <v>0.1</v>
+      </c>
+      <c r="I47" t="s">
+        <v>613</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>349</v>
       </c>
       <c r="B48" t="s">
         <v>350</v>
       </c>
+      <c r="C48" t="s">
+        <v>487</v>
+      </c>
       <c r="D48">
         <v>1</v>
       </c>
-      <c r="G48" s="1"/>
-      <c r="H48" s="1"/>
-    </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="E48" t="s">
+        <v>614</v>
+      </c>
+      <c r="F48" t="s">
+        <v>615</v>
+      </c>
+      <c r="G48" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="H48" s="1">
+        <f t="shared" si="1"/>
+        <v>0.1</v>
+      </c>
+      <c r="I48" t="s">
+        <v>616</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>354</v>
       </c>
       <c r="B49" t="s">
         <v>355</v>
       </c>
+      <c r="C49" t="s">
+        <v>487</v>
+      </c>
       <c r="D49">
         <v>1</v>
       </c>
-      <c r="G49" s="1"/>
-      <c r="H49" s="1"/>
-    </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="E49" t="s">
+        <v>617</v>
+      </c>
+      <c r="F49" t="s">
+        <v>618</v>
+      </c>
+      <c r="G49" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="H49" s="1">
+        <f t="shared" si="1"/>
+        <v>0.1</v>
+      </c>
+      <c r="I49" t="s">
+        <v>619</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>359</v>
       </c>
       <c r="B50" t="s">
         <v>360</v>
       </c>
+      <c r="C50" t="s">
+        <v>487</v>
+      </c>
       <c r="D50">
         <v>1</v>
       </c>
-      <c r="G50" s="1"/>
-      <c r="H50" s="1"/>
-    </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="E50" t="s">
+        <v>620</v>
+      </c>
+      <c r="F50" t="s">
+        <v>621</v>
+      </c>
+      <c r="G50" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="H50" s="1">
+        <f t="shared" si="1"/>
+        <v>0.1</v>
+      </c>
+      <c r="I50" t="s">
+        <v>622</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>364</v>
       </c>
       <c r="B51" t="s">
         <v>365</v>
       </c>
+      <c r="C51" t="s">
+        <v>487</v>
+      </c>
       <c r="D51">
         <v>1</v>
       </c>
-      <c r="G51" s="1"/>
-      <c r="H51" s="1"/>
-    </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="E51" t="s">
+        <v>623</v>
+      </c>
+      <c r="F51" t="s">
+        <v>624</v>
+      </c>
+      <c r="G51" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="H51" s="1">
+        <f t="shared" si="1"/>
+        <v>0.1</v>
+      </c>
+      <c r="I51" t="s">
+        <v>625</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>369</v>
       </c>
       <c r="B52" t="s">
         <v>370</v>
       </c>
+      <c r="C52" t="s">
+        <v>487</v>
+      </c>
       <c r="D52">
         <v>1</v>
       </c>
-      <c r="G52" s="1"/>
-      <c r="H52" s="1"/>
-    </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="E52" t="s">
+        <v>626</v>
+      </c>
+      <c r="F52" t="s">
+        <v>627</v>
+      </c>
+      <c r="G52" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="H52" s="1">
+        <f t="shared" si="1"/>
+        <v>0.1</v>
+      </c>
+      <c r="I52" t="s">
+        <v>628</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>374</v>
       </c>
       <c r="B53" t="s">
         <v>375</v>
       </c>
+      <c r="C53" t="s">
+        <v>487</v>
+      </c>
       <c r="D53">
         <v>1</v>
       </c>
-      <c r="G53" s="1"/>
-      <c r="H53" s="1"/>
-    </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="E53" t="s">
+        <v>629</v>
+      </c>
+      <c r="F53" t="s">
+        <v>630</v>
+      </c>
+      <c r="G53" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="H53" s="1">
+        <f t="shared" si="1"/>
+        <v>0.1</v>
+      </c>
+      <c r="I53" t="s">
+        <v>631</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>379</v>
       </c>
       <c r="B54" t="s">
         <v>380</v>
       </c>
+      <c r="C54" t="s">
+        <v>487</v>
+      </c>
       <c r="D54">
         <v>7</v>
       </c>
-      <c r="G54" s="1"/>
-      <c r="H54" s="1"/>
-    </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="E54" t="s">
+        <v>632</v>
+      </c>
+      <c r="F54" t="s">
+        <v>633</v>
+      </c>
+      <c r="G54" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="H54" s="1">
+        <f t="shared" si="1"/>
+        <v>0.70000000000000007</v>
+      </c>
+      <c r="I54" t="s">
+        <v>634</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>384</v>
       </c>
       <c r="B55" t="s">
         <v>385</v>
       </c>
+      <c r="C55" t="s">
+        <v>487</v>
+      </c>
       <c r="D55">
         <v>1</v>
       </c>
-      <c r="G55" s="1"/>
-      <c r="H55" s="1"/>
-    </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="E55" t="s">
+        <v>635</v>
+      </c>
+      <c r="F55" t="s">
+        <v>636</v>
+      </c>
+      <c r="G55" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="H55" s="1">
+        <f t="shared" si="1"/>
+        <v>0.1</v>
+      </c>
+      <c r="I55" t="s">
+        <v>637</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>404</v>
       </c>
       <c r="B56" t="s">
         <v>405</v>
       </c>
+      <c r="C56" t="s">
+        <v>487</v>
+      </c>
       <c r="D56">
         <v>1</v>
       </c>
-      <c r="G56" s="1"/>
-      <c r="H56" s="1"/>
-    </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="E56" t="s">
+        <v>638</v>
+      </c>
+      <c r="F56" t="s">
+        <v>639</v>
+      </c>
+      <c r="G56" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="H56" s="1">
+        <f t="shared" si="1"/>
+        <v>0.1</v>
+      </c>
+      <c r="I56" t="s">
+        <v>640</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>413</v>
       </c>
       <c r="B57" t="s">
         <v>414</v>
       </c>
+      <c r="C57" t="s">
+        <v>487</v>
+      </c>
       <c r="D57">
         <v>1</v>
       </c>
-      <c r="G57" s="1"/>
-      <c r="H57" s="1"/>
+      <c r="E57" t="s">
+        <v>641</v>
+      </c>
+      <c r="F57" t="s">
+        <v>642</v>
+      </c>
+      <c r="G57" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="H57" s="1">
+        <f t="shared" si="1"/>
+        <v>0.1</v>
+      </c>
+      <c r="I57" t="s">
+        <v>643</v>
+      </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Re-organized Sub-bass and Bass part of the PCB
</commit_message>
<xml_diff>
--- a/Documents/Music_Visualizer_BOM.xlsx
+++ b/Documents/Music_Visualizer_BOM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ECE_Projects\Music_Visualizer\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9E37690-304C-434F-AB0F-477897FE129F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1298627B-B041-45E0-8303-361480EDC5BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Music_Visualizer_BOM" sheetId="1" r:id="rId1"/>
@@ -2821,8 +2821,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I93"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7192,8 +7192,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68457E54-D772-4DE5-8294-89212320B20A}">
   <dimension ref="A1:I57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
-      <selection activeCell="G60" sqref="G60"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B54" sqref="B54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7256,7 +7256,7 @@
         <v>0.1</v>
       </c>
       <c r="H2" s="1">
-        <f>D2*G2</f>
+        <f t="shared" ref="H2:H13" si="0">D2*G2</f>
         <v>0.2</v>
       </c>
       <c r="I2" t="s">
@@ -7286,7 +7286,7 @@
         <v>0.1</v>
       </c>
       <c r="H3" s="1">
-        <f>D3*G3</f>
+        <f t="shared" si="0"/>
         <v>0.2</v>
       </c>
       <c r="I3" t="s">
@@ -7316,7 +7316,7 @@
         <v>0.1</v>
       </c>
       <c r="H4" s="1">
-        <f>D4*G4</f>
+        <f t="shared" si="0"/>
         <v>0.2</v>
       </c>
       <c r="I4" t="s">
@@ -7346,7 +7346,7 @@
         <v>0.1</v>
       </c>
       <c r="H5" s="1">
-        <f>D5*G5</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="I5" t="s">
@@ -7376,7 +7376,7 @@
         <v>0.1</v>
       </c>
       <c r="H6" s="1">
-        <f>D6*G6</f>
+        <f t="shared" si="0"/>
         <v>0.1</v>
       </c>
       <c r="I6" t="s">
@@ -7406,7 +7406,7 @@
         <v>0.1</v>
       </c>
       <c r="H7" s="1">
-        <f>D7*G7</f>
+        <f t="shared" si="0"/>
         <v>0.1</v>
       </c>
       <c r="I7" t="s">
@@ -7436,7 +7436,7 @@
         <v>0.1</v>
       </c>
       <c r="H8" s="1">
-        <f>D8*G8</f>
+        <f t="shared" si="0"/>
         <v>0.1</v>
       </c>
       <c r="I8" t="s">
@@ -7466,7 +7466,7 @@
         <v>0.1</v>
       </c>
       <c r="H9" s="1">
-        <f>D9*G9</f>
+        <f t="shared" si="0"/>
         <v>0.1</v>
       </c>
       <c r="I9" t="s">
@@ -7496,7 +7496,7 @@
         <v>0.1</v>
       </c>
       <c r="H10" s="1">
-        <f>D10*G10</f>
+        <f t="shared" si="0"/>
         <v>0.1</v>
       </c>
       <c r="I10" t="s">
@@ -7526,7 +7526,7 @@
         <v>0.1</v>
       </c>
       <c r="H11" s="1">
-        <f>D11*G11</f>
+        <f t="shared" si="0"/>
         <v>0.1</v>
       </c>
       <c r="I11" t="s">
@@ -7556,7 +7556,7 @@
         <v>0.1</v>
       </c>
       <c r="H12" s="1">
-        <f>D12*G12</f>
+        <f t="shared" si="0"/>
         <v>0.1</v>
       </c>
       <c r="I12" t="s">
@@ -7586,7 +7586,7 @@
         <v>0.1</v>
       </c>
       <c r="H13" s="1">
-        <f>D13*G13</f>
+        <f t="shared" si="0"/>
         <v>0.1</v>
       </c>
       <c r="I13" t="s">
@@ -7616,7 +7616,7 @@
         <v>0.1</v>
       </c>
       <c r="H14" s="1">
-        <f t="shared" ref="H14:H26" si="0">D14*G14</f>
+        <f t="shared" ref="H14:H25" si="1">D14*G14</f>
         <v>0.4</v>
       </c>
       <c r="I14" t="s">
@@ -7646,7 +7646,7 @@
         <v>0.1</v>
       </c>
       <c r="H15" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.1</v>
       </c>
       <c r="I15" t="s">
@@ -7676,7 +7676,7 @@
         <v>0.1</v>
       </c>
       <c r="H16" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.30000000000000004</v>
       </c>
       <c r="I16" t="s">
@@ -7706,7 +7706,7 @@
         <v>0.1</v>
       </c>
       <c r="H17" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.1</v>
       </c>
       <c r="I17" t="s">
@@ -7736,7 +7736,7 @@
         <v>0.1</v>
       </c>
       <c r="H18" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.1</v>
       </c>
       <c r="I18" t="s">
@@ -7766,7 +7766,7 @@
         <v>0.1</v>
       </c>
       <c r="H19" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.30000000000000004</v>
       </c>
       <c r="I19" t="s">
@@ -7796,7 +7796,7 @@
         <v>0.1</v>
       </c>
       <c r="H20" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.1</v>
       </c>
       <c r="I20" t="s">
@@ -7826,7 +7826,7 @@
         <v>0.1</v>
       </c>
       <c r="H21" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.1</v>
       </c>
       <c r="I21" t="s">
@@ -7856,7 +7856,7 @@
         <v>0.1</v>
       </c>
       <c r="H22" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.1</v>
       </c>
       <c r="I22" t="s">
@@ -7886,7 +7886,7 @@
         <v>0.1</v>
       </c>
       <c r="H23" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.1</v>
       </c>
       <c r="I23" t="s">
@@ -7916,7 +7916,7 @@
         <v>0.1</v>
       </c>
       <c r="H24" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.1</v>
       </c>
       <c r="I24" t="s">
@@ -7946,7 +7946,7 @@
         <v>0.1</v>
       </c>
       <c r="H25" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.1</v>
       </c>
       <c r="I25" t="s">
@@ -8036,7 +8036,7 @@
         <v>0.1</v>
       </c>
       <c r="H28" s="1">
-        <f t="shared" ref="H28:H57" si="1">D28*G28</f>
+        <f t="shared" ref="H28:H57" si="2">D28*G28</f>
         <v>0.1</v>
       </c>
       <c r="I28" t="s">
@@ -8066,7 +8066,7 @@
         <v>0.1</v>
       </c>
       <c r="H29" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.1</v>
       </c>
       <c r="I29" t="s">
@@ -8096,7 +8096,7 @@
         <v>0.1</v>
       </c>
       <c r="H30" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.2</v>
       </c>
       <c r="I30" t="s">
@@ -8126,7 +8126,7 @@
         <v>0.1</v>
       </c>
       <c r="H31" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.1</v>
       </c>
       <c r="I31" t="s">
@@ -8156,7 +8156,7 @@
         <v>0.1</v>
       </c>
       <c r="H32" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.1</v>
       </c>
       <c r="I32" t="s">
@@ -8186,7 +8186,7 @@
         <v>0.1</v>
       </c>
       <c r="H33" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.2</v>
       </c>
       <c r="I33" t="s">
@@ -8216,7 +8216,7 @@
         <v>0.1</v>
       </c>
       <c r="H34" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.30000000000000004</v>
       </c>
       <c r="I34" t="s">
@@ -8246,7 +8246,7 @@
         <v>0.1</v>
       </c>
       <c r="H35" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.1</v>
       </c>
       <c r="I35" t="s">
@@ -8276,7 +8276,7 @@
         <v>0.1</v>
       </c>
       <c r="H36" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.1</v>
       </c>
       <c r="I36" t="s">
@@ -8306,7 +8306,7 @@
         <v>0.1</v>
       </c>
       <c r="H37" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.1</v>
       </c>
       <c r="I37" t="s">
@@ -8336,7 +8336,7 @@
         <v>0.1</v>
       </c>
       <c r="H38" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.1</v>
       </c>
       <c r="I38" t="s">
@@ -8366,7 +8366,7 @@
         <v>0.1</v>
       </c>
       <c r="H39" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.1</v>
       </c>
       <c r="I39" t="s">
@@ -8396,7 +8396,7 @@
         <v>0.1</v>
       </c>
       <c r="H40" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.1</v>
       </c>
       <c r="I40" t="s">
@@ -8426,7 +8426,7 @@
         <v>0.1</v>
       </c>
       <c r="H41" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.1</v>
       </c>
       <c r="I41" t="s">
@@ -8456,7 +8456,7 @@
         <v>0.1</v>
       </c>
       <c r="H42" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.1</v>
       </c>
       <c r="I42" t="s">
@@ -8486,7 +8486,7 @@
         <v>0.1</v>
       </c>
       <c r="H43" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.2</v>
       </c>
       <c r="I43" t="s">
@@ -8516,7 +8516,7 @@
         <v>0.1</v>
       </c>
       <c r="H44" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.1</v>
       </c>
       <c r="I44" t="s">
@@ -8546,7 +8546,7 @@
         <v>0.1</v>
       </c>
       <c r="H45" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.1</v>
       </c>
       <c r="I45" t="s">
@@ -8576,7 +8576,7 @@
         <v>0.1</v>
       </c>
       <c r="H46" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.1</v>
       </c>
       <c r="I46" t="s">
@@ -8606,7 +8606,7 @@
         <v>0.1</v>
       </c>
       <c r="H47" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.1</v>
       </c>
       <c r="I47" t="s">
@@ -8636,7 +8636,7 @@
         <v>0.1</v>
       </c>
       <c r="H48" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.1</v>
       </c>
       <c r="I48" t="s">
@@ -8666,7 +8666,7 @@
         <v>0.1</v>
       </c>
       <c r="H49" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.1</v>
       </c>
       <c r="I49" t="s">
@@ -8696,7 +8696,7 @@
         <v>0.1</v>
       </c>
       <c r="H50" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.1</v>
       </c>
       <c r="I50" t="s">
@@ -8726,7 +8726,7 @@
         <v>0.1</v>
       </c>
       <c r="H51" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.1</v>
       </c>
       <c r="I51" t="s">
@@ -8756,7 +8756,7 @@
         <v>0.1</v>
       </c>
       <c r="H52" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.1</v>
       </c>
       <c r="I52" t="s">
@@ -8786,7 +8786,7 @@
         <v>0.1</v>
       </c>
       <c r="H53" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.1</v>
       </c>
       <c r="I53" t="s">
@@ -8816,7 +8816,7 @@
         <v>0.1</v>
       </c>
       <c r="H54" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.70000000000000007</v>
       </c>
       <c r="I54" t="s">
@@ -8846,7 +8846,7 @@
         <v>0.1</v>
       </c>
       <c r="H55" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.1</v>
       </c>
       <c r="I55" t="s">
@@ -8876,7 +8876,7 @@
         <v>0.1</v>
       </c>
       <c r="H56" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.1</v>
       </c>
       <c r="I56" t="s">
@@ -8906,7 +8906,7 @@
         <v>0.1</v>
       </c>
       <c r="H57" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.1</v>
       </c>
       <c r="I57" t="s">

</xml_diff>